<commit_message>
se logra enviar los correos
</commit_message>
<xml_diff>
--- a/jefaturas_template.xlsx
+++ b/jefaturas_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria.yeguez\Documents\GitHub\phishing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB775CB-A156-4939-9256-56CDD5167B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84ABF263-708D-46B9-9AE5-2B21655C01DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -88,9 +88,6 @@
     <t>https://academia.ejemplo.cl/phishing</t>
   </si>
   <si>
-    <t>SeguridadTI@clarovtr.cl</t>
-  </si>
-  <si>
     <t>Jesus Salinas, Matias Rios, Katherine Villalobos</t>
   </si>
   <si>
@@ -107,6 +104,9 @@
   </si>
   <si>
     <t>JF3</t>
+  </si>
+  <si>
+    <t>mariavyeguezp@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -489,8 +489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -504,7 +504,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -562,13 +562,13 @@
       <c r="I2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J2" t="s">
-        <v>22</v>
+      <c r="J2" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -591,13 +591,13 @@
       <c r="H3" t="s">
         <v>20</v>
       </c>
-      <c r="J3" t="s">
-        <v>22</v>
+      <c r="J3" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -606,13 +606,13 @@
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4">
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G4" t="s">
         <v>19</v>
@@ -620,13 +620,15 @@
       <c r="H4" t="s">
         <v>20</v>
       </c>
-      <c r="J4" t="s">
-        <v>22</v>
+      <c r="J4" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="J2" r:id="rId2" xr:uid="{C97B5FC8-F648-492B-8C0A-FBD9DABDCF92}"/>
+    <hyperlink ref="J3:J4" r:id="rId3" display="mariavyeguezp@gmail.com" xr:uid="{668B55A0-254E-49E5-804A-DE89931A4409}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
omite los correos repetidos
</commit_message>
<xml_diff>
--- a/jefaturas_template.xlsx
+++ b/jefaturas_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria.yeguez\Documents\GitHub\phishing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84ABF263-708D-46B9-9AE5-2B21655C01DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFFE109-19FC-4DD4-B989-7EC4E7676F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>jefe_nombre</t>
   </si>
@@ -56,15 +56,6 @@
   </si>
   <si>
     <t>Daniela Ruiz</t>
-  </si>
-  <si>
-    <t>carolina.perez@empresa.cl</t>
-  </si>
-  <si>
-    <t>rodrigo.mella@empresa.cl</t>
-  </si>
-  <si>
-    <t>daniela.ruiz@empresa.cl</t>
   </si>
   <si>
     <t>Juan Soto, Ana Díaz</t>
@@ -489,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -504,7 +495,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -536,92 +527,92 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
         <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
       </c>
       <c r="E2">
         <v>2</v>
       </c>
       <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" t="s">
-        <v>20</v>
-      </c>
       <c r="I2" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
         <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
-        <v>14</v>
+      <c r="C4" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E4">
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -629,6 +620,8 @@
     <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="J2" r:id="rId2" xr:uid="{C97B5FC8-F648-492B-8C0A-FBD9DABDCF92}"/>
     <hyperlink ref="J3:J4" r:id="rId3" display="mariavyeguezp@gmail.com" xr:uid="{668B55A0-254E-49E5-804A-DE89931A4409}"/>
+    <hyperlink ref="C2" r:id="rId4" xr:uid="{2DEFCAEC-55EC-4DC5-AB37-A892EB79CAA3}"/>
+    <hyperlink ref="C3:C4" r:id="rId5" display="mariavyeguezp@gmail.com" xr:uid="{F1F0F0FB-D893-47C8-B18C-6BEEDFD8274F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>